<commit_message>
Removed highlighting to render tables correctly in Markdown
</commit_message>
<xml_diff>
--- a/input/Supplemental_Figure2_data.xlsx
+++ b/input/Supplemental_Figure2_data.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lazarch2/Library/Caches/Cleanup At Startup/com.fetchsoftworks.Fetch/Fetch Temporary Folder 11/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lazarch2/Library/Caches/Cleanup At Startup/com.fetchsoftworks.Fetch/Fetch Temporary Folder 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC31CB2-5982-304C-9C49-47752E937C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F121A2F1-A8E7-3E40-9DEC-76B23DAF7B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1880" yWindow="1740" windowWidth="27700" windowHeight="16320" activeTab="3" xr2:uid="{AE45B9ED-4885-3642-9E60-AEB6EB873DEC}"/>
+    <workbookView xWindow="1880" yWindow="1740" windowWidth="27700" windowHeight="16320" activeTab="4" xr2:uid="{AE45B9ED-4885-3642-9E60-AEB6EB873DEC}"/>
   </bookViews>
   <sheets>
     <sheet name="ETS2_mRNA" sheetId="1" r:id="rId1"/>
     <sheet name="STAT3_protein" sheetId="3" r:id="rId2"/>
     <sheet name="STAT5B_protein" sheetId="4" r:id="rId3"/>
     <sheet name="IL2_mRNA_new_data" sheetId="5" r:id="rId4"/>
-    <sheet name="ETS2_protein_new_data" sheetId="8" r:id="rId5"/>
-    <sheet name="STAT5B_protein_new_data" sheetId="9" r:id="rId6"/>
+    <sheet name="IL2_mRNA_new_data_20250725" sheetId="10" r:id="rId5"/>
+    <sheet name="ETS2_protein_new_data" sheetId="8" r:id="rId6"/>
+    <sheet name="STAT5B_protein_new_data" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="22">
   <si>
     <t>condition</t>
   </si>
@@ -2346,8 +2347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16089102-A2CD-5841-BD35-970DC2AA7A5A}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23:E25"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2711,6 +2712,478 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FFEFB3-16A3-5642-8789-51E08D80A7C9}">
+  <dimension ref="A1:E41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>1.1723329425556858E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>1.452081316553727E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>2.0387359836901122E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>1.7235E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>1.5789999999999998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>1.4489795918367347</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>1.4519119351100811</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>1.5771065182829889</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10">
+        <v>1.4689030000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>1.4972399999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12">
+        <v>1.2161458333333333</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13">
+        <v>1.6234756097560976</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14">
+        <v>1.6670918367346939</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15">
+        <v>1.51834</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16">
+        <v>1.4989319999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17">
+        <v>1.5392354124748491</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18">
+        <v>1.6887661141804788</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19">
+        <v>0.83524355300859598</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20">
+        <v>1.3466899999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21">
+        <v>1.3502050000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22">
+        <v>0.55284552845528456</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23">
+        <v>0.27899846704138986</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24">
+        <v>0.47662018047579985</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25">
+        <v>0.43502299999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26">
+        <v>0.44575799999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27">
+        <v>0.52277904328018221</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28">
+        <v>0.69108910891089104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29">
+        <v>0.48097826086956524</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30">
+        <v>0.56643200000000005</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31">
+        <v>0.55998099999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32">
+        <v>0.24482248520710059</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33">
+        <v>0.18401332223147376</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34">
+        <v>0.42870036101083031</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35">
+        <v>0.32413999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36">
+        <v>0.27825499999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37">
+        <v>0.11313591495823842</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38">
+        <v>0.18695306284805091</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39">
+        <v>0.13944817300521997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40">
+        <v>0.14099</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41">
+        <v>0.13988500000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D71BB0EE-964E-6A40-A29F-A96FEDB403D5}">
   <dimension ref="A1:D57"/>
   <sheetViews>
@@ -3523,7 +3996,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B276293-15E0-E143-A4B4-2175B6B7751E}">
   <dimension ref="A1:D57"/>
   <sheetViews>

</xml_diff>